<commit_message>
Add codes for leave-one-out sensitivity analysis
</commit_message>
<xml_diff>
--- a/data-auroc.xlsx
+++ b/data-auroc.xlsx
@@ -79,10 +79,10 @@
     <t>Timóteo et al.</t>
   </si>
   <si>
-    <t>Yang et al. (A)</t>
-  </si>
-  <si>
-    <t>Yang et al. (B)</t>
+    <t>Yang et al. (non-DM)</t>
+  </si>
+  <si>
+    <t>Yang et al. (DM)</t>
   </si>
   <si>
     <t>Qin et al.</t>
@@ -93,7 +93,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +117,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -212,7 +218,7 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">

</xml_diff>